<commit_message>
combined documents together, conclusion needs rework
</commit_message>
<xml_diff>
--- a/Analysis Codes/Experimental Data Reorganized.xlsx
+++ b/Analysis Codes/Experimental Data Reorganized.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\J lab\Final Project\Analysis Codes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ME201617\ME Spring 2017\Final project\Analysis Codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="30">
   <si>
     <t>RPM</t>
   </si>
@@ -100,6 +100,21 @@
   </si>
   <si>
     <t>TRIAL 4</t>
+  </si>
+  <si>
+    <t>&lt;-Water Density</t>
+  </si>
+  <si>
+    <t>Accuracies</t>
+  </si>
+  <si>
+    <t>Error in Pdyn</t>
+  </si>
+  <si>
+    <t>Error ratio</t>
+  </si>
+  <si>
+    <t>Error</t>
   </si>
 </sst>
 </file>
@@ -1007,10 +1022,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V45"/>
+  <dimension ref="A1:AB45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9:V15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z17" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,9 +1089,7 @@
       <c r="M2" s="15"/>
       <c r="N2" s="15"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -1122,13 +1135,6 @@
       </c>
       <c r="O3" s="20" t="s">
         <v>20</v>
-      </c>
-      <c r="P3" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q3">
-        <f xml:space="preserve"> 1.2093</f>
-        <v>1.2093</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -1734,7 +1740,7 @@
       </c>
     </row>
     <row r="16" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B17" s="32" t="s">
         <v>3</v>
       </c>
@@ -1754,7 +1760,7 @@
       <c r="N17" s="88"/>
       <c r="O17" s="89"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B18" s="35" t="s">
         <v>15</v>
       </c>
@@ -1794,7 +1800,7 @@
       </c>
       <c r="O18" s="93"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B19" s="39">
         <v>1.65</v>
       </c>
@@ -1842,7 +1848,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B20" s="39">
         <v>2</v>
       </c>
@@ -1871,8 +1877,11 @@
         <v>3.17</v>
       </c>
       <c r="O20" s="70"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="T20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B21" s="39">
         <v>2.4500000000000002</v>
       </c>
@@ -1905,8 +1914,20 @@
         <v>1.65</v>
       </c>
       <c r="O21" s="70"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S21" t="s">
+        <v>14</v>
+      </c>
+      <c r="T21">
+        <v>1.2093</v>
+      </c>
+      <c r="U21">
+        <v>1000</v>
+      </c>
+      <c r="V21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B22" s="39">
         <v>3</v>
       </c>
@@ -1951,8 +1972,11 @@
       <c r="O22" s="45" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B23" s="43">
         <v>1.65</v>
       </c>
@@ -1987,8 +2011,26 @@
         <v>21</v>
       </c>
       <c r="O23" s="82"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="S23">
+        <v>0.05</v>
+      </c>
+      <c r="T23">
+        <v>0.05</v>
+      </c>
+      <c r="U23">
+        <v>0.05</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B24" s="43">
         <v>2</v>
       </c>
@@ -2017,8 +2059,41 @@
         <v>21</v>
       </c>
       <c r="O24" s="25"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R24">
+        <v>12.009733090745195</v>
+      </c>
+      <c r="S24">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="T24">
+        <v>3.0303030303030307E-2</v>
+      </c>
+      <c r="U24">
+        <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="V24">
+        <v>9.1827614554637312E-4</v>
+      </c>
+      <c r="W24">
+        <v>1.4792924408284025E-3</v>
+      </c>
+      <c r="X24">
+        <v>169033.71499640998</v>
+      </c>
+      <c r="Y24">
+        <v>104928.18304644</v>
+      </c>
+      <c r="Z24">
+        <v>17.619281945775914</v>
+      </c>
+      <c r="AA24">
+        <v>0.1010153658876122</v>
+      </c>
+      <c r="AB24">
+        <v>1.2131675823741896</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B25" s="43">
         <v>2.4500000000000002</v>
       </c>
@@ -2063,8 +2138,41 @@
       <c r="O25" s="73" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R25">
+        <v>16.366507419737342</v>
+      </c>
+      <c r="S25">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="T25">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="U25">
+        <v>3.7037037037037035E-2</v>
+      </c>
+      <c r="V25">
+        <v>6.2500250000000011E-4</v>
+      </c>
+      <c r="W25">
+        <v>1.3717446124828531E-3</v>
+      </c>
+      <c r="X25">
+        <v>248350.72910400003</v>
+      </c>
+      <c r="Y25">
+        <v>113154.80094801002</v>
+      </c>
+      <c r="Z25">
+        <v>17.619288156558007</v>
+      </c>
+      <c r="AA25">
+        <v>5.4392908497546695E-2</v>
+      </c>
+      <c r="AB25">
+        <v>0.8902219405061923</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B26" s="43">
         <v>3</v>
       </c>
@@ -2097,8 +2205,41 @@
         <v>21.92</v>
       </c>
       <c r="O26" s="74"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R26">
+        <v>19.786142659186879</v>
+      </c>
+      <c r="S26">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="T26">
+        <v>2.0408163265306121E-2</v>
+      </c>
+      <c r="U26">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="V26">
+        <v>4.1649562786339015E-4</v>
+      </c>
+      <c r="W26">
+        <v>1.1111136111111111E-3</v>
+      </c>
+      <c r="X26">
+        <v>372681.31286169006</v>
+      </c>
+      <c r="Y26">
+        <v>139697.28512099996</v>
+      </c>
+      <c r="Z26">
+        <v>17.619298860241145</v>
+      </c>
+      <c r="AA26">
+        <v>3.7216223159722124E-2</v>
+      </c>
+      <c r="AB26">
+        <v>0.73636550067439666</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B27" s="47">
         <v>1.65</v>
       </c>
@@ -2133,8 +2274,41 @@
         <v>13.91</v>
       </c>
       <c r="O27" s="84"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R27">
+        <v>24.019466181490394</v>
+      </c>
+      <c r="S27">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="T27">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="U27">
+        <v>3.125E-2</v>
+      </c>
+      <c r="V27">
+        <v>2.7778027777777776E-4</v>
+      </c>
+      <c r="W27">
+        <v>9.7656499999999999E-4</v>
+      </c>
+      <c r="X27">
+        <v>558789.14048399986</v>
+      </c>
+      <c r="Y27">
+        <v>158944.46662656005</v>
+      </c>
+      <c r="Z27">
+        <v>17.619313429132752</v>
+      </c>
+      <c r="AA27">
+        <v>2.5253886597221151E-2</v>
+      </c>
+      <c r="AB27">
+        <v>0.60658487507314696</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B28" s="47">
         <v>2</v>
       </c>
@@ -2176,7 +2350,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B29" s="47">
         <v>2.4500000000000002</v>
       </c>
@@ -2210,7 +2384,7 @@
       </c>
       <c r="O29" s="28"/>
     </row>
-    <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="51">
         <v>3</v>
       </c>
@@ -2244,7 +2418,7 @@
       </c>
       <c r="O30" s="31"/>
     </row>
-    <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2252,7 +2426,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B32" s="54" t="s">
         <v>1</v>
       </c>

</xml_diff>